<commit_message>
Making changes to the Product and Sprint Backlog to better represent the requirements of this sprint
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -31,16 +31,7 @@
     <t>EFFORT ESTIMATION</t>
   </si>
   <si>
-    <t>As a user, I want to see the contributions towards a particular file in the form of a pie chart</t>
-  </si>
-  <si>
-    <t>Representation of contribution/Interface</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a user, I want access to contribution data through a web based application </t>
+    <t xml:space="preserve">As a user with permission to a particular file, I want access to contribution data through a web based application </t>
   </si>
   <si>
     <t>Platform</t>
@@ -49,34 +40,22 @@
     <t>XS</t>
   </si>
   <si>
-    <t>As a user, I want to be able to see the actions taken by other users part of that Drive folder so as to know which actions they have contributed</t>
-  </si>
-  <si>
-    <t>Action used to make changes</t>
-  </si>
-  <si>
-    <t>XL</t>
-  </si>
-  <si>
-    <t>As a user, I want the interface to look neat and clean so that I can look at and understand the contents with ease</t>
-  </si>
-  <si>
-    <t>Interface</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>As a user, I want to access the app through google authentication so that I can access my drive's files</t>
-  </si>
-  <si>
-    <t>Authentication/Log In</t>
-  </si>
-  <si>
     <t xml:space="preserve">As a developer, I need to be able to connect to Google Drive API </t>
   </si>
   <si>
     <t>Data retrieval from Drive using Drive API</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>As a developer, I need to use the OAuth 2.0 protocol to authenticate users</t>
+  </si>
+  <si>
+    <t>Authentication/Log in</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
   <si>
     <t>As a developer, I need to be able to use the API to get the ID of a change</t>
@@ -89,6 +68,42 @@
   </si>
   <si>
     <t>As a developer, I need to be able to retrieve the changes that a user has made to a file</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>As a user, I need to see changes to a file in chronological order in the form of a timeline provided I have permission to access that file</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>As a user, I want to access the app through google authentication so that I can access my drive's files</t>
+  </si>
+  <si>
+    <t>Authentication/Log In</t>
+  </si>
+  <si>
+    <t>As a user with many team drives, I want to select what team drive to display data, for so my screen does not get clogged up</t>
+  </si>
+  <si>
+    <t>As a user with permission to a particular file, I want to see the contributions towards that file in the form of a pie chart</t>
+  </si>
+  <si>
+    <t>Representation of contribution/Interface</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to see the actions taken by other users part of that Drive folder so as to know which actions they have contributed</t>
+  </si>
+  <si>
+    <t>Action used to make changes</t>
+  </si>
+  <si>
+    <t>As a user, I want the interface to look neat and clean so that I can look at and understand the contents with ease</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -106,10 +121,10 @@
     </font>
     <font/>
     <font>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -194,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -227,10 +242,7 @@
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -239,11 +251,8 @@
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -324,7 +333,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="10">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>7</v>
@@ -343,7 +352,7 @@
       <c r="C6" s="10">
         <v>1.0</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -358,7 +367,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="10">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>13</v>
@@ -374,14 +383,14 @@
       <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="12">
-        <v>9.0</v>
+      <c r="C8" s="10">
+        <v>2.0</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -389,16 +398,16 @@
         <v>5.0</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>19</v>
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -406,16 +415,16 @@
         <v>6.0</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>21</v>
+        <v>4.0</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -423,16 +432,16 @@
         <v>7.0</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>21</v>
+        <v>5.0</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -440,16 +449,16 @@
         <v>8.0</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="D12" s="13" t="s">
+        <v>5.0</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -457,52 +466,85 @@
         <v>9.0</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="C14" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="14">
-        <v>10.0</v>
-      </c>
-      <c r="B14" s="15" t="s">
+      <c r="E14" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="D14" s="17" t="s">
+      <c r="C15" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="13">
+        <v>13.0</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="15">
+        <v>9.0</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5"/>
@@ -6395,12 +6437,6 @@
       <c r="C999" s="5"/>
       <c r="D999" s="5"/>
       <c r="E999" s="5"/>
-    </row>
-    <row r="1000">
-      <c r="A1000" s="5"/>
-      <c r="C1000" s="5"/>
-      <c r="D1000" s="5"/>
-      <c r="E1000" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
The documentation for SPRINT 3
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -37,16 +37,13 @@
     <t>Platform</t>
   </si>
   <si>
-    <t>XS</t>
+    <t>M</t>
   </si>
   <si>
     <t xml:space="preserve">As a developer, I need to be able to connect to Google Drive API </t>
   </si>
   <si>
     <t>Data retrieval from Drive using Drive API</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>As a developer, I need to use the OAuth 2.0 protocol to authenticate users</t>
@@ -61,16 +58,31 @@
     <t>As a developer, I need to be able to use the API to get the ID of a change</t>
   </si>
   <si>
+    <t>As a user, I need to be able to see the individual changes data for a file represented in the form of a histogram</t>
+  </si>
+  <si>
+    <t>Graphical Representation</t>
+  </si>
+  <si>
+    <t>As a user, I need to be able to see the revision data being represented in the form of a pie chart</t>
+  </si>
+  <si>
+    <t>As a user, I need to be able to see the revision data for files within a team drive, even when a folder exists in said drive</t>
+  </si>
+  <si>
+    <t>As a developer, I need to be able to retrieve the files inside a folder</t>
+  </si>
+  <si>
     <t>As a developer, I need to be able to use the API to get the time of change</t>
   </si>
   <si>
-    <t>As a developer, I need to be able to use the API to get the name of the user who made the change</t>
+    <t>As a developer, I need to be able to retrieve the number of actions that a user has made to a file</t>
   </si>
   <si>
-    <t>As a developer, I need to be able to retrieve the changes that a user has made to a file</t>
+    <t>Data retrieval</t>
   </si>
   <si>
-    <t>XL</t>
+    <t>As a developer, I need to be able to use the API to get the name of the user who made the change</t>
   </si>
   <si>
     <t>As a user, I need to see changes to a file in chronological order in the form of a timeline provided I have permission to access that file</t>
@@ -100,10 +112,31 @@
     <t>Action used to make changes</t>
   </si>
   <si>
+    <t>XL</t>
+  </si>
+  <si>
     <t>As a user, I want the interface to look neat and clean so that I can look at and understand the contents with ease</t>
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I need to be able to see the revision information on a webpage </t>
+  </si>
+  <si>
+    <t>Printing data on the webpage</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Formatting</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -128,7 +161,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,12 +170,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF9FC5E8"/>
+        <bgColor rgb="FF9FC5E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border/>
     <border>
       <left style="thin">
@@ -205,11 +244,25 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -230,32 +283,74 @@
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="9" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -356,7 +451,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -364,24 +459,24 @@
         <v>3.0</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="10">
         <v>1.0</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="10">
         <v>2.0</v>
@@ -390,191 +485,246 @@
         <v>10</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="B9" s="9" t="s">
+        <v>6.0</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>10</v>
-      </c>
       <c r="E9" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8">
-        <v>6.0</v>
-      </c>
-      <c r="B10" s="9" t="s">
+        <v>7.0</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="16">
+        <v>8.0</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="18">
+        <v>2.0</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="8">
-        <v>7.0</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>19</v>
+      <c r="E11" s="19" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8">
-        <v>8.0</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>11</v>
+        <v>9.0</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>23</v>
+        <v>3.0</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" s="10">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>26</v>
+        <v>4.0</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="10">
+      <c r="E17" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="10">
         <v>8.0</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="13">
-        <v>13.0</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="15">
+      <c r="D20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8">
+        <v>18.0</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="21">
         <v>9.0</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="A22" s="22">
+        <v>19.0</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="24">
+        <v>10.0</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5"/>
@@ -583,19 +733,29 @@
       <c r="E23" s="5"/>
     </row>
     <row r="24">
-      <c r="A24" s="5"/>
+      <c r="A24" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25">
-      <c r="A25" s="5"/>
+      <c r="A25" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>40</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26">
-      <c r="A26" s="5"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="30" t="s">
+        <v>41</v>
+      </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -6437,6 +6597,12 @@
       <c r="C999" s="5"/>
       <c r="D999" s="5"/>
       <c r="E999" s="5"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="5"/>
+      <c r="C1000" s="5"/>
+      <c r="D1000" s="5"/>
+      <c r="E1000" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>